<commit_message>
Fix FED SB/BATS in SIT.
</commit_message>
<xml_diff>
--- a/msit_feds.xlsx
+++ b/msit_feds.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$1:$K$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$1:$K$245</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="981">
   <si>
     <r>
       <rPr>
@@ -12255,6 +12255,88 @@
   </si>
   <si>
     <t>11-12(24)/5-6(12)</t>
+  </si>
+  <si>
+    <t>—NA—</t>
+  </si>
+  <si>
+    <t>F&amp;E</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12(12)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>◆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/
+6(6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>◆</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>36(24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>◆</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/
+18(12)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>◆</t>
+    </r>
+  </si>
+  <si>
+    <t>Y181</t>
   </si>
 </sst>
 </file>
@@ -12266,7 +12348,7 @@
     <numFmt numFmtId="165" formatCode="###0.0;###0.0"/>
     <numFmt numFmtId="166" formatCode="###0.00;###0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -12308,6 +12390,11 @@
       <sz val="9"/>
       <name val="MS Gothic"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -12434,7 +12521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -12534,6 +12621,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12597,7 +12696,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12901,10 +13000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K243"/>
+  <dimension ref="A1:K245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="F212" sqref="F212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12958,10 +13057,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -13083,10 +13182,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -13524,7 +13623,7 @@
       <c r="B20" s="16">
         <v>32</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="33" t="s">
         <v>974</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -13588,11 +13687,11 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -13743,10 +13842,10 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -14663,10 +14762,10 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -14769,8 +14868,8 @@
       <c r="G58" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="H58" s="8" t="s">
-        <v>272</v>
+      <c r="H58" s="34" t="s">
+        <v>975</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>273</v>
@@ -15136,11 +15235,11 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="34"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="38"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -15431,102 +15530,102 @@
       </c>
     </row>
     <row r="79" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="36" t="s">
+      <c r="A79" s="40" t="s">
         <v>357</v>
       </c>
-      <c r="B79" s="39">
+      <c r="B79" s="43">
         <v>111</v>
       </c>
-      <c r="C79" s="42" t="s">
+      <c r="C79" s="46" t="s">
         <v>358</v>
       </c>
-      <c r="D79" s="36" t="s">
+      <c r="D79" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E79" s="44">
+      <c r="E79" s="48">
         <v>8</v>
       </c>
-      <c r="F79" s="36" t="s">
+      <c r="F79" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="G79" s="36" t="s">
+      <c r="G79" s="40" t="s">
         <v>319</v>
       </c>
       <c r="H79" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I79" s="36" t="s">
+      <c r="I79" s="40" t="s">
         <v>360</v>
       </c>
-      <c r="J79" s="47">
+      <c r="J79" s="51">
         <v>1.8</v>
       </c>
-      <c r="K79" s="36" t="s">
+      <c r="K79" s="40" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="45"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="37"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="49"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
       <c r="H80" s="25" t="s">
         <v>362</v>
       </c>
-      <c r="I80" s="37"/>
-      <c r="J80" s="48"/>
-      <c r="K80" s="37"/>
+      <c r="I80" s="41"/>
+      <c r="J80" s="52"/>
+      <c r="K80" s="41"/>
     </row>
     <row r="81" spans="1:11" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="37"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="37"/>
-      <c r="G81" s="37"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
       <c r="H81" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="I81" s="37"/>
-      <c r="J81" s="48"/>
-      <c r="K81" s="37"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="52"/>
+      <c r="K81" s="41"/>
     </row>
     <row r="82" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="37"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="37"/>
+      <c r="A82" s="41"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="47"/>
+      <c r="D82" s="41"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="41"/>
+      <c r="G82" s="41"/>
       <c r="H82" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="I82" s="37"/>
-      <c r="J82" s="48"/>
-      <c r="K82" s="37"/>
+      <c r="I82" s="41"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="41"/>
     </row>
     <row r="83" spans="1:11" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="38"/>
-      <c r="B83" s="41"/>
+      <c r="A83" s="42"/>
+      <c r="B83" s="45"/>
       <c r="C83" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="D83" s="38"/>
-      <c r="E83" s="46"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="38"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="42"/>
       <c r="H83" s="28" t="s">
         <v>366</v>
       </c>
       <c r="I83" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="J83" s="49"/>
+      <c r="J83" s="53"/>
       <c r="K83" s="28" t="s">
         <v>368</v>
       </c>
@@ -15707,11 +15806,11 @@
       </c>
     </row>
     <row r="89" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="33" t="s">
+      <c r="A89" s="37" t="s">
         <v>390</v>
       </c>
-      <c r="B89" s="35"/>
-      <c r="C89" s="34"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="38"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -16453,10 +16552,10 @@
       </c>
     </row>
     <row r="111" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="33" t="s">
+      <c r="A111" s="37" t="s">
         <v>475</v>
       </c>
-      <c r="B111" s="34"/>
+      <c r="B111" s="38"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -16818,11 +16917,11 @@
       </c>
     </row>
     <row r="122" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="33" t="s">
+      <c r="A122" s="37" t="s">
         <v>526</v>
       </c>
-      <c r="B122" s="35"/>
-      <c r="C122" s="34"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="38"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
@@ -16973,10 +17072,10 @@
       </c>
     </row>
     <row r="127" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="33" t="s">
+      <c r="A127" s="37" t="s">
         <v>545</v>
       </c>
-      <c r="B127" s="34"/>
+      <c r="B127" s="38"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -17233,11 +17332,11 @@
       </c>
     </row>
     <row r="135" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="33" t="s">
+      <c r="A135" s="37" t="s">
         <v>572</v>
       </c>
-      <c r="B135" s="35"/>
-      <c r="C135" s="34"/>
+      <c r="B135" s="39"/>
+      <c r="C135" s="38"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
@@ -17528,11 +17627,11 @@
       </c>
     </row>
     <row r="144" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="33" t="s">
+      <c r="A144" s="37" t="s">
         <v>607</v>
       </c>
-      <c r="B144" s="35"/>
-      <c r="C144" s="34"/>
+      <c r="B144" s="39"/>
+      <c r="C144" s="38"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
@@ -18083,10 +18182,10 @@
       </c>
     </row>
     <row r="161" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="33" t="s">
+      <c r="A161" s="37" t="s">
         <v>675</v>
       </c>
-      <c r="B161" s="34"/>
+      <c r="B161" s="38"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -18203,11 +18302,11 @@
       </c>
     </row>
     <row r="165" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="33" t="s">
+      <c r="A165" s="37" t="s">
         <v>693</v>
       </c>
-      <c r="B165" s="35"/>
-      <c r="C165" s="34"/>
+      <c r="B165" s="39"/>
+      <c r="C165" s="38"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
       <c r="F165" s="4"/>
@@ -18286,10 +18385,10 @@
       </c>
     </row>
     <row r="168" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="33" t="s">
+      <c r="A168" s="37" t="s">
         <v>698</v>
       </c>
-      <c r="B168" s="34"/>
+      <c r="B168" s="38"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -18371,19 +18470,19 @@
       </c>
     </row>
     <row r="171" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="50" t="s">
+      <c r="A171" s="54" t="s">
         <v>708</v>
       </c>
-      <c r="B171" s="50"/>
-      <c r="C171" s="50"/>
-      <c r="D171" s="50"/>
-      <c r="E171" s="50"/>
-      <c r="F171" s="50"/>
-      <c r="G171" s="50"/>
-      <c r="H171" s="50"/>
-      <c r="I171" s="50"/>
-      <c r="J171" s="50"/>
-      <c r="K171" s="50"/>
+      <c r="B171" s="54"/>
+      <c r="C171" s="54"/>
+      <c r="D171" s="54"/>
+      <c r="E171" s="54"/>
+      <c r="F171" s="54"/>
+      <c r="G171" s="54"/>
+      <c r="H171" s="54"/>
+      <c r="I171" s="54"/>
+      <c r="J171" s="54"/>
+      <c r="K171" s="54"/>
     </row>
     <row r="172" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
@@ -18526,19 +18625,19 @@
       </c>
     </row>
     <row r="176" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="50" t="s">
+      <c r="A176" s="54" t="s">
         <v>726</v>
       </c>
-      <c r="B176" s="50"/>
-      <c r="C176" s="50"/>
-      <c r="D176" s="50"/>
-      <c r="E176" s="50"/>
-      <c r="F176" s="50"/>
-      <c r="G176" s="50"/>
-      <c r="H176" s="50"/>
-      <c r="I176" s="50"/>
-      <c r="J176" s="50"/>
-      <c r="K176" s="50"/>
+      <c r="B176" s="54"/>
+      <c r="C176" s="54"/>
+      <c r="D176" s="54"/>
+      <c r="E176" s="54"/>
+      <c r="F176" s="54"/>
+      <c r="G176" s="54"/>
+      <c r="H176" s="54"/>
+      <c r="I176" s="54"/>
+      <c r="J176" s="54"/>
+      <c r="K176" s="54"/>
     </row>
     <row r="177" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
@@ -18556,19 +18655,19 @@
       <c r="K177" s="11"/>
     </row>
     <row r="178" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="50" t="s">
+      <c r="A178" s="54" t="s">
         <v>727</v>
       </c>
-      <c r="B178" s="50"/>
-      <c r="C178" s="50"/>
-      <c r="D178" s="50"/>
-      <c r="E178" s="50"/>
-      <c r="F178" s="50"/>
-      <c r="G178" s="50"/>
-      <c r="H178" s="50"/>
-      <c r="I178" s="50"/>
-      <c r="J178" s="50"/>
-      <c r="K178" s="50"/>
+      <c r="B178" s="54"/>
+      <c r="C178" s="54"/>
+      <c r="D178" s="54"/>
+      <c r="E178" s="54"/>
+      <c r="F178" s="54"/>
+      <c r="G178" s="54"/>
+      <c r="H178" s="54"/>
+      <c r="I178" s="54"/>
+      <c r="J178" s="54"/>
+      <c r="K178" s="54"/>
     </row>
     <row r="179" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="8" t="s">
@@ -18851,19 +18950,19 @@
       </c>
     </row>
     <row r="187" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="50" t="s">
+      <c r="A187" s="54" t="s">
         <v>767</v>
       </c>
-      <c r="B187" s="50"/>
-      <c r="C187" s="50"/>
-      <c r="D187" s="50"/>
-      <c r="E187" s="50"/>
-      <c r="F187" s="50"/>
-      <c r="G187" s="50"/>
-      <c r="H187" s="50"/>
-      <c r="I187" s="50"/>
-      <c r="J187" s="50"/>
-      <c r="K187" s="50"/>
+      <c r="B187" s="54"/>
+      <c r="C187" s="54"/>
+      <c r="D187" s="54"/>
+      <c r="E187" s="54"/>
+      <c r="F187" s="54"/>
+      <c r="G187" s="54"/>
+      <c r="H187" s="54"/>
+      <c r="I187" s="54"/>
+      <c r="J187" s="54"/>
+      <c r="K187" s="54"/>
     </row>
     <row r="188" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="s">
@@ -19041,19 +19140,19 @@
       </c>
     </row>
     <row r="193" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="50" t="s">
+      <c r="A193" s="54" t="s">
         <v>793</v>
       </c>
-      <c r="B193" s="50"/>
-      <c r="C193" s="50"/>
-      <c r="D193" s="50"/>
-      <c r="E193" s="50"/>
-      <c r="F193" s="50"/>
-      <c r="G193" s="50"/>
-      <c r="H193" s="50"/>
-      <c r="I193" s="50"/>
-      <c r="J193" s="50"/>
-      <c r="K193" s="50"/>
+      <c r="B193" s="54"/>
+      <c r="C193" s="54"/>
+      <c r="D193" s="54"/>
+      <c r="E193" s="54"/>
+      <c r="F193" s="54"/>
+      <c r="G193" s="54"/>
+      <c r="H193" s="54"/>
+      <c r="I193" s="54"/>
+      <c r="J193" s="54"/>
+      <c r="K193" s="54"/>
     </row>
     <row r="194" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="s">
@@ -19441,19 +19540,19 @@
       </c>
     </row>
     <row r="205" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="50" t="s">
+      <c r="A205" s="54" t="s">
         <v>841</v>
       </c>
-      <c r="B205" s="50"/>
-      <c r="C205" s="50"/>
-      <c r="D205" s="50"/>
-      <c r="E205" s="50"/>
-      <c r="F205" s="50"/>
-      <c r="G205" s="50"/>
-      <c r="H205" s="50"/>
-      <c r="I205" s="50"/>
-      <c r="J205" s="50"/>
-      <c r="K205" s="50"/>
+      <c r="B205" s="54"/>
+      <c r="C205" s="54"/>
+      <c r="D205" s="54"/>
+      <c r="E205" s="54"/>
+      <c r="F205" s="54"/>
+      <c r="G205" s="54"/>
+      <c r="H205" s="54"/>
+      <c r="I205" s="54"/>
+      <c r="J205" s="54"/>
+      <c r="K205" s="54"/>
     </row>
     <row r="206" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="8" t="s">
@@ -19596,19 +19695,19 @@
       </c>
     </row>
     <row r="210" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="50" t="s">
+      <c r="A210" s="54" t="s">
         <v>863</v>
       </c>
-      <c r="B210" s="50"/>
-      <c r="C210" s="50"/>
-      <c r="D210" s="50"/>
-      <c r="E210" s="50"/>
-      <c r="F210" s="50"/>
-      <c r="G210" s="50"/>
-      <c r="H210" s="50"/>
-      <c r="I210" s="50"/>
-      <c r="J210" s="50"/>
-      <c r="K210" s="50"/>
+      <c r="B210" s="54"/>
+      <c r="C210" s="54"/>
+      <c r="D210" s="54"/>
+      <c r="E210" s="54"/>
+      <c r="F210" s="54"/>
+      <c r="G210" s="54"/>
+      <c r="H210" s="54"/>
+      <c r="I210" s="54"/>
+      <c r="J210" s="54"/>
+      <c r="K210" s="54"/>
     </row>
     <row r="211" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="8" t="s">
@@ -19652,17 +19751,17 @@
       <c r="B212" s="7">
         <v>2</v>
       </c>
-      <c r="C212" s="11" t="s">
-        <v>871</v>
-      </c>
-      <c r="D212" s="5" t="s">
-        <v>30</v>
+      <c r="C212" s="36" t="s">
+        <v>978</v>
+      </c>
+      <c r="D212" s="35" t="s">
+        <v>976</v>
       </c>
       <c r="E212" s="7">
         <v>9</v>
       </c>
-      <c r="F212" s="5" t="s">
-        <v>809</v>
+      <c r="F212" s="35" t="s">
+        <v>980</v>
       </c>
       <c r="G212" s="5" t="s">
         <v>872</v>
@@ -19680,310 +19779,310 @@
         <v>874</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="8" t="s">
+    <row r="213" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="B213" s="7">
+        <v>2</v>
+      </c>
+      <c r="C213" s="11" t="s">
+        <v>871</v>
+      </c>
+      <c r="D213" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E213" s="7">
+        <v>9</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="G213" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="H213" s="11" t="s">
+        <v>873</v>
+      </c>
+      <c r="I213" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="J213" s="9">
+        <v>0</v>
+      </c>
+      <c r="K213" s="5" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="8" t="s">
         <v>875</v>
       </c>
-      <c r="B213" s="10">
+      <c r="B214" s="10">
         <v>24</v>
       </c>
-      <c r="C213" s="20" t="s">
+      <c r="C214" s="20" t="s">
         <v>876</v>
       </c>
-      <c r="D213" s="8" t="s">
+      <c r="D214" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E213" s="12">
+      <c r="E214" s="12">
         <v>6</v>
       </c>
-      <c r="F213" s="8" t="s">
+      <c r="F214" s="8" t="s">
         <v>844</v>
       </c>
-      <c r="G213" s="8" t="s">
+      <c r="G214" s="8" t="s">
         <v>877</v>
       </c>
-      <c r="H213" s="8" t="s">
+      <c r="H214" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I213" s="8" t="s">
+      <c r="I214" s="8" t="s">
         <v>846</v>
       </c>
-      <c r="J213" s="14">
+      <c r="J214" s="14">
         <v>0</v>
       </c>
-      <c r="K213" s="8" t="s">
+      <c r="K214" s="8" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="5" t="s">
+    <row r="215" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="B214" s="5" t="s">
+      <c r="B215" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="C214" s="20" t="s">
+      <c r="C215" s="58" t="s">
+        <v>979</v>
+      </c>
+      <c r="D215" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E215" s="7">
+        <v>10</v>
+      </c>
+      <c r="F215" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="G215" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="H215" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="I215" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="J215" s="9">
+        <v>0</v>
+      </c>
+      <c r="K215" s="11" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="C216" s="20" t="s">
         <v>881</v>
       </c>
-      <c r="D214" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E214" s="7">
+      <c r="D216" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E216" s="7">
         <v>10</v>
       </c>
-      <c r="F214" s="5" t="s">
+      <c r="F216" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G214" s="5" t="s">
+      <c r="G216" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="H214" s="5" t="s">
+      <c r="H216" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="I214" s="5" t="s">
+      <c r="I216" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="J214" s="9">
+      <c r="J216" s="9">
         <v>0</v>
       </c>
-      <c r="K214" s="11" t="s">
+      <c r="K216" s="11" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="215" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A215" s="8" t="s">
+    <row r="217" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="8" t="s">
         <v>885</v>
       </c>
-      <c r="B215" s="12">
+      <c r="B217" s="12">
         <v>4</v>
       </c>
-      <c r="C215" s="11" t="s">
+      <c r="C217" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="D215" s="8" t="s">
+      <c r="D217" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E215" s="12">
+      <c r="E217" s="12">
         <v>0</v>
       </c>
-      <c r="F215" s="8" t="s">
+      <c r="F217" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G215" s="8" t="s">
+      <c r="G217" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H215" s="8" t="s">
+      <c r="H217" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I215" s="8" t="s">
+      <c r="I217" s="8" t="s">
         <v>887</v>
       </c>
-      <c r="J215" s="14">
+      <c r="J217" s="14">
         <v>0</v>
       </c>
-      <c r="K215" s="8" t="s">
+      <c r="K217" s="8" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A216" s="8" t="s">
+    <row r="218" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="8" t="s">
         <v>889</v>
       </c>
-      <c r="B216" s="8" t="s">
+      <c r="B218" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="C216" s="13" t="s">
+      <c r="C218" s="13" t="s">
         <v>890</v>
       </c>
-      <c r="D216" s="8" t="s">
+      <c r="D218" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E216" s="12">
+      <c r="E218" s="12">
         <v>0</v>
       </c>
-      <c r="F216" s="8" t="s">
+      <c r="F218" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G216" s="8" t="s">
+      <c r="G218" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H216" s="8" t="s">
+      <c r="H218" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I216" s="8" t="s">
+      <c r="I218" s="8" t="s">
         <v>891</v>
       </c>
-      <c r="J216" s="14">
+      <c r="J218" s="14">
         <v>0</v>
       </c>
-      <c r="K216" s="8" t="s">
+      <c r="K218" s="8" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="5" t="s">
+    <row r="219" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="B217" s="6">
+      <c r="B219" s="6">
         <v>47</v>
       </c>
-      <c r="C217" s="11" t="s">
+      <c r="C219" s="11" t="s">
         <v>893</v>
       </c>
-      <c r="D217" s="5" t="s">
+      <c r="D219" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E217" s="7">
+      <c r="E219" s="7">
         <v>9</v>
       </c>
-      <c r="F217" s="5" t="s">
+      <c r="F219" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G217" s="5" t="s">
+      <c r="G219" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="H217" s="8" t="s">
+      <c r="H219" s="8" t="s">
         <v>895</v>
       </c>
-      <c r="I217" s="5" t="s">
+      <c r="I219" s="5" t="s">
         <v>896</v>
-      </c>
-      <c r="J217" s="9">
-        <v>0</v>
-      </c>
-      <c r="K217" s="5" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="218" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="11" t="s">
-        <v>898</v>
-      </c>
-      <c r="B218" s="6">
-        <v>17</v>
-      </c>
-      <c r="C218" s="19" t="s">
-        <v>899</v>
-      </c>
-      <c r="D218" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E218" s="6">
-        <v>0</v>
-      </c>
-      <c r="F218" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G218" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="H218" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I218" s="5" t="s">
-        <v>900</v>
-      </c>
-      <c r="J218" s="9">
-        <v>0</v>
-      </c>
-      <c r="K218" s="5" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="219" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="5" t="s">
-        <v>902</v>
-      </c>
-      <c r="B219" s="6">
-        <v>202</v>
-      </c>
-      <c r="C219" s="11" t="s">
-        <v>903</v>
-      </c>
-      <c r="D219" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E219" s="7">
-        <v>10</v>
-      </c>
-      <c r="F219" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G219" s="5" t="s">
-        <v>904</v>
-      </c>
-      <c r="H219" s="11" t="s">
-        <v>905</v>
-      </c>
-      <c r="I219" s="5" t="s">
-        <v>272</v>
       </c>
       <c r="J219" s="9">
         <v>0</v>
       </c>
       <c r="K219" s="5" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="220" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="B220" s="6">
+        <v>17</v>
+      </c>
+      <c r="C220" s="19" t="s">
+        <v>899</v>
+      </c>
+      <c r="D220" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E220" s="6">
         <v>0</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G220" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H220" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I220" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J220" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K220" s="1" t="s">
+      <c r="F220" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G220" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H220" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I220" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="J220" s="9">
+        <v>0</v>
+      </c>
+      <c r="K220" s="5" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="B221" s="6">
+        <v>202</v>
+      </c>
+      <c r="C221" s="11" t="s">
+        <v>903</v>
+      </c>
+      <c r="D221" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E221" s="7">
         <v>10</v>
-      </c>
-    </row>
-    <row r="221" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="5" t="s">
-        <v>907</v>
-      </c>
-      <c r="B221" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="C221" s="11" t="s">
-        <v>909</v>
-      </c>
-      <c r="D221" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E221" s="7">
-        <v>9</v>
       </c>
       <c r="F221" s="5" t="s">
         <v>113</v>
       </c>
       <c r="G221" s="5" t="s">
-        <v>867</v>
+        <v>904</v>
       </c>
       <c r="H221" s="11" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="I221" s="5" t="s">
         <v>272</v>
@@ -19992,319 +20091,339 @@
         <v>0</v>
       </c>
       <c r="K221" s="5" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="222" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="5" t="s">
-        <v>911</v>
-      </c>
-      <c r="B222" s="6">
-        <v>201</v>
-      </c>
-      <c r="C222" s="20" t="s">
-        <v>912</v>
-      </c>
-      <c r="D222" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E222" s="7">
-        <v>11</v>
-      </c>
-      <c r="F222" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G222" s="5" t="s">
-        <v>882</v>
-      </c>
-      <c r="H222" s="11" t="s">
-        <v>913</v>
-      </c>
-      <c r="I222" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="J222" s="9">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K222" s="5" t="s">
-        <v>914</v>
+      <c r="B222" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H222" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I222" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J222" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K222" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="223" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
-        <v>915</v>
-      </c>
-      <c r="B223" s="8" t="s">
-        <v>916</v>
+        <v>907</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>908</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="D223" s="5" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="E223" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F223" s="5" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G223" s="5" t="s">
-        <v>894</v>
+        <v>867</v>
       </c>
       <c r="H223" s="11" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="I223" s="5" t="s">
-        <v>896</v>
+        <v>272</v>
       </c>
       <c r="J223" s="9">
         <v>0</v>
       </c>
       <c r="K223" s="5" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="B224" s="6">
+        <v>201</v>
+      </c>
+      <c r="C224" s="20" t="s">
+        <v>912</v>
+      </c>
+      <c r="D224" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E224" s="7">
+        <v>11</v>
+      </c>
+      <c r="F224" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G224" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="H224" s="11" t="s">
+        <v>913</v>
+      </c>
+      <c r="I224" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="J224" s="9">
+        <v>0</v>
+      </c>
+      <c r="K224" s="5" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>916</v>
+      </c>
+      <c r="C225" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="D225" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E225" s="7">
+        <v>10</v>
+      </c>
+      <c r="F225" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G225" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="H225" s="11" t="s">
+        <v>918</v>
+      </c>
+      <c r="I225" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="J225" s="9">
+        <v>0</v>
+      </c>
+      <c r="K225" s="5" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="8" t="s">
+    <row r="226" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="8" t="s">
         <v>920</v>
       </c>
-      <c r="B224" s="11"/>
-      <c r="C224" s="11"/>
-      <c r="D224" s="11"/>
-      <c r="E224" s="11"/>
-      <c r="F224" s="11"/>
-      <c r="G224" s="11"/>
-      <c r="H224" s="11"/>
-      <c r="I224" s="11"/>
-      <c r="J224" s="11"/>
-      <c r="K224" s="8" t="s">
+      <c r="B226" s="11"/>
+      <c r="C226" s="11"/>
+      <c r="D226" s="11"/>
+      <c r="E226" s="11"/>
+      <c r="F226" s="11"/>
+      <c r="G226" s="11"/>
+      <c r="H226" s="11"/>
+      <c r="I226" s="11"/>
+      <c r="J226" s="11"/>
+      <c r="K226" s="8" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="50" t="s">
+    <row r="227" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="54" t="s">
         <v>922</v>
       </c>
-      <c r="B225" s="50"/>
-      <c r="C225" s="50"/>
-      <c r="D225" s="50"/>
-      <c r="E225" s="50"/>
-      <c r="F225" s="50"/>
-      <c r="G225" s="50"/>
-      <c r="H225" s="50"/>
-      <c r="I225" s="50"/>
-      <c r="J225" s="50"/>
-      <c r="K225" s="50"/>
-    </row>
-    <row r="226" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="5" t="s">
+      <c r="B227" s="54"/>
+      <c r="C227" s="54"/>
+      <c r="D227" s="54"/>
+      <c r="E227" s="54"/>
+      <c r="F227" s="54"/>
+      <c r="G227" s="54"/>
+      <c r="H227" s="54"/>
+      <c r="I227" s="54"/>
+      <c r="J227" s="54"/>
+      <c r="K227" s="54"/>
+    </row>
+    <row r="228" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="B226" s="6">
+      <c r="B228" s="6">
         <v>14</v>
       </c>
-      <c r="C226" s="5" t="s">
+      <c r="C228" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="D226" s="5" t="s">
+      <c r="D228" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E226" s="7">
+      <c r="E228" s="7">
         <v>0</v>
       </c>
-      <c r="F226" s="5" t="s">
+      <c r="F228" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="G226" s="5" t="s">
+      <c r="G228" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H226" s="5" t="s">
+      <c r="H228" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="I226" s="11" t="s">
+      <c r="I228" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="J226" s="9">
+      <c r="J228" s="9">
         <v>0</v>
       </c>
-      <c r="K226" s="5" t="s">
+      <c r="K228" s="5" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="8" t="s">
+    <row r="229" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="8" t="s">
         <v>927</v>
       </c>
-      <c r="B227" s="8" t="s">
+      <c r="B229" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="C227" s="8" t="s">
+      <c r="C229" s="8" t="s">
         <v>928</v>
       </c>
-      <c r="D227" s="8" t="s">
+      <c r="D229" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="E227" s="12">
+      <c r="E229" s="12">
         <v>0</v>
       </c>
-      <c r="F227" s="8" t="s">
+      <c r="F229" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="G227" s="8" t="s">
+      <c r="G229" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H227" s="8" t="s">
+      <c r="H229" s="8" t="s">
         <v>929</v>
       </c>
-      <c r="I227" s="8" t="s">
+      <c r="I229" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="J227" s="14">
+      <c r="J229" s="14">
         <v>0</v>
       </c>
-      <c r="K227" s="8" t="s">
+      <c r="K229" s="8" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="8" t="s">
+    <row r="230" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="8" t="s">
         <v>931</v>
       </c>
-      <c r="B228" s="8" t="s">
+      <c r="B230" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="C228" s="8" t="s">
+      <c r="C230" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="D228" s="8" t="s">
+      <c r="D230" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="E228" s="12">
+      <c r="E230" s="12">
         <v>0</v>
       </c>
-      <c r="F228" s="8" t="s">
+      <c r="F230" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="G228" s="8" t="s">
+      <c r="G230" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H228" s="8" t="s">
+      <c r="H230" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I228" s="8" t="s">
+      <c r="I230" s="8" t="s">
         <v>932</v>
       </c>
-      <c r="J228" s="14">
+      <c r="J230" s="14">
         <v>0</v>
       </c>
-      <c r="K228" s="8" t="s">
+      <c r="K230" s="8" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="5" t="s">
+    <row r="231" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="B229" s="6">
+      <c r="B231" s="6">
         <v>14</v>
       </c>
-      <c r="C229" s="5" t="s">
+      <c r="C231" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="D229" s="5" t="s">
+      <c r="D231" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E229" s="7">
+      <c r="E231" s="7">
         <v>0</v>
       </c>
-      <c r="F229" s="5" t="s">
+      <c r="F231" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G229" s="5" t="s">
+      <c r="G231" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H229" s="5" t="s">
+      <c r="H231" s="5" t="s">
         <v>936</v>
       </c>
-      <c r="I229" s="11" t="s">
+      <c r="I231" s="11" t="s">
         <v>937</v>
       </c>
-      <c r="J229" s="9">
+      <c r="J231" s="9">
         <v>0</v>
       </c>
-      <c r="K229" s="5" t="s">
+      <c r="K231" s="5" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A230" s="5" t="s">
-        <v>939</v>
-      </c>
-      <c r="B230" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C230" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="D230" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="E230" s="7">
-        <v>0</v>
-      </c>
-      <c r="F230" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="G230" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="H230" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I230" s="5" t="s">
-        <v>940</v>
-      </c>
-      <c r="J230" s="9">
-        <v>0</v>
-      </c>
-      <c r="K230" s="5" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="231" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="50" t="s">
-        <v>942</v>
-      </c>
-      <c r="B231" s="50"/>
-      <c r="C231" s="50"/>
-      <c r="D231" s="50"/>
-      <c r="E231" s="50"/>
-      <c r="F231" s="50"/>
-      <c r="G231" s="50"/>
-      <c r="H231" s="50"/>
-      <c r="I231" s="50"/>
-      <c r="J231" s="50"/>
-      <c r="K231" s="50"/>
     </row>
     <row r="232" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="5" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>944</v>
+        <v>21</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>943</v>
+        <v>269</v>
       </c>
       <c r="D232" s="5" t="s">
-        <v>97</v>
+        <v>640</v>
       </c>
       <c r="E232" s="7">
         <v>0</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>730</v>
+        <v>685</v>
       </c>
       <c r="G232" s="5" t="s">
         <v>272</v>
@@ -20313,138 +20432,118 @@
         <v>272</v>
       </c>
       <c r="I232" s="5" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="J232" s="9">
         <v>0</v>
       </c>
       <c r="K232" s="5" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="54" t="s">
+        <v>942</v>
+      </c>
+      <c r="B233" s="54"/>
+      <c r="C233" s="54"/>
+      <c r="D233" s="54"/>
+      <c r="E233" s="54"/>
+      <c r="F233" s="54"/>
+      <c r="G233" s="54"/>
+      <c r="H233" s="54"/>
+      <c r="I233" s="54"/>
+      <c r="J233" s="54"/>
+      <c r="K233" s="54"/>
+    </row>
+    <row r="234" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="5" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A233" s="5" t="s">
-        <v>946</v>
-      </c>
-      <c r="B233" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="C233" s="19" t="s">
-        <v>946</v>
-      </c>
-      <c r="D233" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E233" s="7">
+      <c r="B234" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="D234" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E234" s="7">
         <v>0</v>
       </c>
-      <c r="F233" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G233" s="5" t="s">
+      <c r="F234" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="G234" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H233" s="5" t="s">
-        <v>799</v>
-      </c>
-      <c r="I233" s="8" t="s">
-        <v>947</v>
-      </c>
-      <c r="J233" s="9">
+      <c r="H234" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I234" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="J234" s="9">
         <v>0</v>
       </c>
-      <c r="K233" s="5" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="234" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="11" t="s">
-        <v>949</v>
-      </c>
-      <c r="B234" s="8" t="s">
-        <v>799</v>
-      </c>
-      <c r="C234" s="11" t="s">
-        <v>949</v>
-      </c>
-      <c r="D234" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E234" s="12">
-        <v>1</v>
-      </c>
-      <c r="F234" s="8" t="s">
-        <v>950</v>
-      </c>
-      <c r="G234" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="H234" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="I234" s="8" t="s">
-        <v>951</v>
-      </c>
-      <c r="J234" s="14">
-        <v>0</v>
-      </c>
-      <c r="K234" s="8" t="s">
-        <v>952</v>
+      <c r="K234" s="5" t="s">
+        <v>943</v>
       </c>
     </row>
     <row r="235" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="5" t="s">
-        <v>953</v>
+        <v>946</v>
       </c>
       <c r="B235" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="C235" s="32" t="s">
-        <v>954</v>
+      <c r="C235" s="19" t="s">
+        <v>946</v>
       </c>
       <c r="D235" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="E235" s="6">
-        <v>1</v>
-      </c>
-      <c r="F235" s="11" t="s">
-        <v>955</v>
+        <v>90</v>
+      </c>
+      <c r="E235" s="7">
+        <v>0</v>
+      </c>
+      <c r="F235" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="G235" s="5" t="s">
         <v>272</v>
       </c>
       <c r="H235" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I235" s="5" t="s">
-        <v>956</v>
+        <v>799</v>
+      </c>
+      <c r="I235" s="8" t="s">
+        <v>947</v>
       </c>
       <c r="J235" s="9">
         <v>0</v>
       </c>
       <c r="K235" s="5" t="s">
-        <v>957</v>
+        <v>948</v>
       </c>
     </row>
     <row r="236" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="8" t="s">
-        <v>958</v>
+      <c r="A236" s="11" t="s">
+        <v>949</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>959</v>
-      </c>
-      <c r="C236" s="8" t="s">
-        <v>960</v>
+        <v>799</v>
+      </c>
+      <c r="C236" s="11" t="s">
+        <v>949</v>
       </c>
       <c r="D236" s="8" t="s">
-        <v>640</v>
+        <v>14</v>
       </c>
       <c r="E236" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F236" s="8" t="s">
-        <v>961</v>
+        <v>950</v>
       </c>
       <c r="G236" s="8" t="s">
         <v>272</v>
@@ -20453,94 +20552,94 @@
         <v>272</v>
       </c>
       <c r="I236" s="8" t="s">
-        <v>962</v>
+        <v>951</v>
       </c>
       <c r="J236" s="14">
         <v>0</v>
       </c>
       <c r="K236" s="8" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="237" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A237" s="8" t="s">
-        <v>964</v>
-      </c>
-      <c r="B237" s="8" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="5" t="s">
+        <v>953</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="C237" s="32" t="s">
+        <v>954</v>
+      </c>
+      <c r="D237" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="E237" s="6">
+        <v>1</v>
+      </c>
+      <c r="F237" s="11" t="s">
+        <v>955</v>
+      </c>
+      <c r="G237" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H237" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I237" s="5" t="s">
+        <v>956</v>
+      </c>
+      <c r="J237" s="9">
+        <v>0</v>
+      </c>
+      <c r="K237" s="5" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="8" t="s">
+        <v>958</v>
+      </c>
+      <c r="B238" s="8" t="s">
         <v>959</v>
       </c>
-      <c r="C237" s="8" t="s">
-        <v>965</v>
-      </c>
-      <c r="D237" s="8" t="s">
+      <c r="C238" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="D238" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="E237" s="12">
+      <c r="E238" s="12">
         <v>0</v>
       </c>
-      <c r="F237" s="8" t="s">
+      <c r="F238" s="8" t="s">
         <v>961</v>
       </c>
-      <c r="G237" s="8" t="s">
+      <c r="G238" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H237" s="8" t="s">
+      <c r="H238" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I237" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="J237" s="14">
+      <c r="I238" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="J238" s="14">
         <v>0</v>
       </c>
-      <c r="K237" s="8" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="238" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A238" s="5" t="s">
-        <v>967</v>
-      </c>
-      <c r="B238" s="5" t="s">
-        <v>959</v>
-      </c>
-      <c r="C238" s="5" t="s">
-        <v>968</v>
-      </c>
-      <c r="D238" s="5" t="s">
-        <v>640</v>
-      </c>
-      <c r="E238" s="7">
-        <v>0</v>
-      </c>
-      <c r="F238" s="5" t="s">
-        <v>961</v>
-      </c>
-      <c r="G238" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="H238" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I238" s="5" t="s">
-        <v>966</v>
-      </c>
-      <c r="J238" s="9">
-        <v>0</v>
-      </c>
-      <c r="K238" s="5" t="s">
+      <c r="K238" s="8" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="239" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="8" t="s">
-        <v>969</v>
+        <v>964</v>
       </c>
       <c r="B239" s="8" t="s">
         <v>959</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>960</v>
+        <v>965</v>
       </c>
       <c r="D239" s="8" t="s">
         <v>640</v>
@@ -20558,7 +20657,7 @@
         <v>272</v>
       </c>
       <c r="I239" s="8" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="J239" s="14">
         <v>0</v>
@@ -20567,44 +20666,44 @@
         <v>963</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A240" s="8" t="s">
-        <v>970</v>
-      </c>
-      <c r="B240" s="8" t="s">
+    <row r="240" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="C240" s="8" t="s">
-        <v>960</v>
-      </c>
-      <c r="D240" s="8" t="s">
+      <c r="C240" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="D240" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="E240" s="12">
+      <c r="E240" s="7">
         <v>0</v>
       </c>
-      <c r="F240" s="8" t="s">
+      <c r="F240" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="G240" s="8" t="s">
+      <c r="G240" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H240" s="8" t="s">
+      <c r="H240" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="I240" s="8" t="s">
-        <v>962</v>
-      </c>
-      <c r="J240" s="14">
+      <c r="I240" s="5" t="s">
+        <v>966</v>
+      </c>
+      <c r="J240" s="9">
         <v>0</v>
       </c>
-      <c r="K240" s="8" t="s">
+      <c r="K240" s="5" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="241" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="8" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B241" s="8" t="s">
         <v>959</v>
@@ -20628,7 +20727,7 @@
         <v>272</v>
       </c>
       <c r="I241" s="8" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="J241" s="14">
         <v>0</v>
@@ -20639,7 +20738,7 @@
     </row>
     <row r="242" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="8" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B242" s="8" t="s">
         <v>959</v>
@@ -20673,27 +20772,97 @@
       </c>
     </row>
     <row r="243" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A243" s="51" t="s">
+      <c r="A243" s="8" t="s">
+        <v>971</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="C243" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="D243" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="E243" s="12">
+        <v>0</v>
+      </c>
+      <c r="F243" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="G243" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H243" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I243" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="J243" s="14">
+        <v>0</v>
+      </c>
+      <c r="K243" s="8" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="8" t="s">
+        <v>972</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>959</v>
+      </c>
+      <c r="C244" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="D244" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="E244" s="12">
+        <v>0</v>
+      </c>
+      <c r="F244" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="G244" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H244" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I244" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="J244" s="14">
+        <v>0</v>
+      </c>
+      <c r="K244" s="8" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="55" t="s">
         <v>973</v>
       </c>
-      <c r="B243" s="52"/>
-      <c r="C243" s="52"/>
-      <c r="D243" s="52"/>
-      <c r="E243" s="52"/>
-      <c r="F243" s="52"/>
-      <c r="G243" s="52"/>
-      <c r="H243" s="52"/>
-      <c r="I243" s="52"/>
-      <c r="J243" s="52"/>
-      <c r="K243" s="53"/>
+      <c r="B245" s="56"/>
+      <c r="C245" s="56"/>
+      <c r="D245" s="56"/>
+      <c r="E245" s="56"/>
+      <c r="F245" s="56"/>
+      <c r="G245" s="56"/>
+      <c r="H245" s="56"/>
+      <c r="I245" s="56"/>
+      <c r="J245" s="56"/>
+      <c r="K245" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="35">
     <mergeCell ref="A205:K205"/>
     <mergeCell ref="A210:K210"/>
-    <mergeCell ref="A225:K225"/>
-    <mergeCell ref="A231:K231"/>
-    <mergeCell ref="A243:K243"/>
+    <mergeCell ref="A227:K227"/>
+    <mergeCell ref="A233:K233"/>
+    <mergeCell ref="A245:K245"/>
     <mergeCell ref="A171:K171"/>
     <mergeCell ref="A176:K176"/>
     <mergeCell ref="A178:K178"/>
@@ -20726,5 +20895,6 @@
     <mergeCell ref="A55:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add MB (ND) to all SITs.
</commit_message>
<xml_diff>
--- a/msit_feds.xlsx
+++ b/msit_feds.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="978">
   <si>
     <t>Designation</t>
   </si>
@@ -4191,6 +4191,15 @@
     </r>
   </si>
   <si>
+    <t>MB (ND)</t>
+  </si>
+  <si>
+    <t>MB(3)</t>
+  </si>
+  <si>
+    <t>Undeployed MB</t>
+  </si>
+  <si>
     <t>MB</t>
   </si>
   <si>
@@ -4217,9 +4226,6 @@
     </r>
   </si>
   <si>
-    <t>MB(3)</t>
-  </si>
-  <si>
     <t>See (510.2); EW=1</t>
   </si>
   <si>
@@ -4230,7 +4236,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">36(24)</t>
+      <t xml:space="preserve">36(18H12)</t>
     </r>
     <r>
       <rPr>
@@ -4249,7 +4255,7 @@
         <sz val="9"/>
       </rPr>
       <t xml:space="preserve">/
-18(12)</t>
+18(9H6)</t>
     </r>
     <r>
       <rPr>
@@ -4270,39 +4276,6 @@
   <si>
     <t>Starbase. See (433.41), (441.0), and
 (510.3)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">36(18H12)</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="MS Gothic"/>
-        <charset val="1"/>
-        <family val="3"/>
-        <sz val="9"/>
-      </rPr>
-      <t xml:space="preserve">◆</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <sz val="9"/>
-      </rPr>
-      <t xml:space="preserve">/
-18(9H6)</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="MS Gothic"/>
-        <charset val="1"/>
-        <family val="3"/>
-        <sz val="9"/>
-      </rPr>
-      <t xml:space="preserve">◆</t>
-    </r>
   </si>
   <si>
     <t>Ftr-Module</t>
@@ -4895,12 +4868,6 @@
       <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="9"/>
-    </font>
-    <font>
       <name val="Times New Roman"/>
       <charset val="204"/>
       <family val="1"/>
@@ -4918,6 +4885,12 @@
       <name val="MS Gothic"/>
       <charset val="1"/>
       <family val="3"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -4947,7 +4920,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
@@ -4956,36 +4929,43 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left style="medium"/>
       <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right/>
       <top style="medium"/>
       <bottom style="medium"/>
       <diagonal/>
@@ -5016,7 +4996,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -5025,11 +5005,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5041,11 +5021,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5053,11 +5033,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5065,7 +5045,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5073,7 +5053,7 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5081,19 +5061,15 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5101,19 +5077,11 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5141,10 +5109,6 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
@@ -5153,19 +5117,39 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5192,8 +5176,8 @@
   </sheetPr>
   <dimension ref="A1:K246"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A53" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B58" activeCellId="0" pane="topLeft" sqref="B58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A210" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A215" activeCellId="0" pane="topLeft" sqref="215:216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5479,13 +5463,13 @@
       <c r="G10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="19" t="n">
+      <c r="J10" s="18" t="n">
         <v>4.8</v>
       </c>
       <c r="K10" s="8" t="s">
@@ -5496,7 +5480,7 @@
       <c r="A11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -5523,7 +5507,7 @@
       <c r="J11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5590,7 +5574,7 @@
       <c r="I13" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="19" t="n">
+      <c r="J13" s="18" t="n">
         <v>4.2</v>
       </c>
       <c r="K13" s="8" t="s">
@@ -5601,10 +5585,10 @@
       <c r="A14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="8" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -5628,7 +5612,7 @@
       <c r="J14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="8" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5639,7 +5623,7 @@
       <c r="B15" s="6" t="n">
         <v>61</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -5654,7 +5638,7 @@
       <c r="G15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="8" t="s">
         <v>74</v>
       </c>
       <c r="I15" s="5" t="s">
@@ -5674,7 +5658,7 @@
       <c r="B16" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -5689,7 +5673,7 @@
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="8" t="s">
         <v>79</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -5709,7 +5693,7 @@
       <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="13" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -5744,7 +5728,7 @@
       <c r="B18" s="6" t="n">
         <v>123</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -5776,10 +5760,10 @@
       <c r="A19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="13" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -5788,7 +5772,7 @@
       <c r="E19" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="8" t="s">
         <v>98</v>
       </c>
       <c r="G19" s="15" t="s">
@@ -5803,7 +5787,7 @@
       <c r="J19" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="8" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5823,22 +5807,22 @@
       <c r="E20" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="8" t="s">
         <v>98</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="8" t="s">
         <v>102</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="19" t="n">
+      <c r="J20" s="18" t="n">
         <v>4.8</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="8" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5899,7 +5883,7 @@
       <c r="B23" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -5914,7 +5898,7 @@
       <c r="G23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="8" t="s">
         <v>109</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -5949,7 +5933,7 @@
       <c r="G24" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="8" t="s">
         <v>115</v>
       </c>
       <c r="I24" s="8" t="s">
@@ -5993,7 +5977,7 @@
       <c r="J25" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="8" t="s">
         <v>122</v>
       </c>
     </row>
@@ -6004,7 +5988,7 @@
       <c r="B26" s="6" t="n">
         <v>64</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>124</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -6089,7 +6073,7 @@
       <c r="B29" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="21" t="s">
         <v>136</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -6104,7 +6088,7 @@
       <c r="G29" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="8" t="s">
         <v>138</v>
       </c>
       <c r="I29" s="5" t="s">
@@ -6124,7 +6108,7 @@
       <c r="B30" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -6142,7 +6126,7 @@
       <c r="H30" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="8" t="s">
         <v>145</v>
       </c>
       <c r="J30" s="9" t="n">
@@ -6159,7 +6143,7 @@
       <c r="B31" s="6" t="n">
         <v>131</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>148</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -6177,7 +6161,7 @@
       <c r="H31" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="8" t="s">
         <v>152</v>
       </c>
       <c r="J31" s="9" t="n">
@@ -6209,10 +6193,10 @@
       <c r="G32" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="I32" s="8" t="s">
         <v>159</v>
       </c>
       <c r="J32" s="9" t="n">
@@ -6229,7 +6213,7 @@
       <c r="B33" s="6" t="n">
         <v>82</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>162</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -6244,7 +6228,7 @@
       <c r="G33" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="8" t="s">
         <v>163</v>
       </c>
       <c r="I33" s="5" t="s">
@@ -6261,7 +6245,7 @@
       <c r="A34" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -6334,7 +6318,7 @@
       <c r="B36" s="6" t="n">
         <v>51</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="21" t="s">
         <v>175</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -6352,7 +6336,7 @@
       <c r="H36" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="8" t="s">
         <v>178</v>
       </c>
       <c r="J36" s="9" t="n">
@@ -6369,7 +6353,7 @@
       <c r="B37" s="16" t="n">
         <v>87</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D37" s="15" t="s">
@@ -6384,16 +6368,16 @@
       <c r="G37" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="H37" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I37" s="18" t="s">
+      <c r="I37" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="J37" s="19" t="n">
+      <c r="J37" s="18" t="n">
         <v>2.4</v>
       </c>
-      <c r="K37" s="18" t="s">
+      <c r="K37" s="8" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6436,10 +6420,10 @@
       <c r="A39" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="13" t="s">
         <v>192</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -6463,7 +6447,7 @@
       <c r="J39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K39" s="18" t="s">
+      <c r="K39" s="8" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6489,10 +6473,10 @@
       <c r="G40" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="8" t="s">
         <v>198</v>
       </c>
       <c r="J40" s="9" t="n">
@@ -6524,10 +6508,10 @@
       <c r="G41" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="18" t="s">
+      <c r="I41" s="8" t="s">
         <v>198</v>
       </c>
       <c r="J41" s="9" t="n">
@@ -6559,7 +6543,7 @@
       <c r="G42" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="8" t="s">
         <v>203</v>
       </c>
       <c r="I42" s="5" t="s">
@@ -6629,7 +6613,7 @@
       <c r="G44" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="8" t="s">
         <v>209</v>
       </c>
       <c r="I44" s="5" t="s">
@@ -6649,7 +6633,7 @@
       <c r="B45" s="10" t="n">
         <v>127</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="22" t="s">
         <v>213</v>
       </c>
       <c r="D45" s="8" t="s">
@@ -6681,7 +6665,7 @@
       <c r="A46" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -6734,7 +6718,7 @@
       <c r="G47" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="8" t="s">
         <v>221</v>
       </c>
       <c r="I47" s="5" t="s">
@@ -6754,7 +6738,7 @@
       <c r="B48" s="16" t="n">
         <v>129</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="21" t="s">
         <v>225</v>
       </c>
       <c r="D48" s="15" t="s">
@@ -6769,13 +6753,13 @@
       <c r="G48" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="8" t="s">
         <v>226</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="J48" s="19" t="n">
+      <c r="J48" s="18" t="n">
         <v>2.4</v>
       </c>
       <c r="K48" s="8" t="s">
@@ -6804,7 +6788,7 @@
       <c r="G49" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="H49" s="8" t="s">
         <v>231</v>
       </c>
       <c r="I49" s="5" t="s">
@@ -6839,7 +6823,7 @@
       <c r="G50" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H50" s="18" t="s">
+      <c r="H50" s="8" t="s">
         <v>236</v>
       </c>
       <c r="I50" s="5" t="s">
@@ -6848,7 +6832,7 @@
       <c r="J50" s="9" t="n">
         <v>2.7</v>
       </c>
-      <c r="K50" s="18" t="s">
+      <c r="K50" s="8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -6859,7 +6843,7 @@
       <c r="B51" s="6" t="n">
         <v>201</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -6874,7 +6858,7 @@
       <c r="G51" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="8" t="s">
         <v>240</v>
       </c>
       <c r="I51" s="5" t="s">
@@ -6894,7 +6878,7 @@
       <c r="B52" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="23" t="s">
         <v>245</v>
       </c>
       <c r="D52" s="15" t="s">
@@ -6909,13 +6893,13 @@
       <c r="G52" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H52" s="24" t="s">
+      <c r="H52" s="5" t="s">
         <v>246</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="J52" s="19" t="n">
+      <c r="J52" s="18" t="n">
         <v>3.6</v>
       </c>
       <c r="K52" s="8" t="s">
@@ -7161,7 +7145,7 @@
       <c r="F61" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="19" t="s">
         <v>266</v>
       </c>
       <c r="H61" s="5" t="s">
@@ -7231,7 +7215,7 @@
       <c r="F63" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="19" t="s">
         <v>266</v>
       </c>
       <c r="H63" s="5" t="s">
@@ -7369,7 +7353,7 @@
       <c r="F67" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="19" t="s">
         <v>266</v>
       </c>
       <c r="H67" s="5" t="s">
@@ -7404,7 +7388,7 @@
       <c r="F68" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="19" t="s">
         <v>266</v>
       </c>
       <c r="H68" s="5" t="s">
@@ -7517,7 +7501,7 @@
       <c r="B73" s="6" t="n">
         <v>106</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="19" t="s">
         <v>325</v>
       </c>
       <c r="D73" s="5" t="s">
@@ -7532,7 +7516,7 @@
       <c r="G73" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H73" s="18" t="s">
+      <c r="H73" s="8" t="s">
         <v>326</v>
       </c>
       <c r="I73" s="5" t="s">
@@ -7567,16 +7551,16 @@
       <c r="G74" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H74" s="18" t="s">
+      <c r="H74" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="I74" s="18" t="s">
+      <c r="I74" s="8" t="s">
         <v>332</v>
       </c>
       <c r="J74" s="9" t="n">
         <v>1.8</v>
       </c>
-      <c r="K74" s="18" t="s">
+      <c r="K74" s="8" t="s">
         <v>333</v>
       </c>
     </row>
@@ -7602,7 +7586,7 @@
       <c r="G75" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="H75" s="8" t="s">
         <v>336</v>
       </c>
       <c r="I75" s="5" t="s">
@@ -7622,7 +7606,7 @@
       <c r="B76" s="6" t="n">
         <v>109</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="19" t="s">
         <v>340</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -7637,7 +7621,7 @@
       <c r="G76" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H76" s="18" t="s">
+      <c r="H76" s="8" t="s">
         <v>341</v>
       </c>
       <c r="I76" s="5" t="s">
@@ -7657,7 +7641,7 @@
       <c r="B77" s="16" t="n">
         <v>110</v>
       </c>
-      <c r="C77" s="23" t="s">
+      <c r="C77" s="21" t="s">
         <v>136</v>
       </c>
       <c r="D77" s="15" t="s">
@@ -7672,13 +7656,13 @@
       <c r="G77" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H77" s="18" t="s">
+      <c r="H77" s="8" t="s">
         <v>344</v>
       </c>
       <c r="I77" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="J77" s="19" t="n">
+      <c r="J77" s="18" t="n">
         <v>1.8</v>
       </c>
       <c r="K77" s="5" t="s">
@@ -7692,7 +7676,7 @@
       <c r="B78" s="6" t="n">
         <v>114</v>
       </c>
-      <c r="C78" s="23" t="s">
+      <c r="C78" s="21" t="s">
         <v>348</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -7707,7 +7691,7 @@
       <c r="G78" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H78" s="18" t="s">
+      <c r="H78" s="8" t="s">
         <v>350</v>
       </c>
       <c r="I78" s="5" t="s">
@@ -7727,7 +7711,7 @@
       <c r="B79" s="6" t="n">
         <v>115</v>
       </c>
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="21" t="s">
         <v>354</v>
       </c>
       <c r="D79" s="5" t="s">
@@ -7742,7 +7726,7 @@
       <c r="G79" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H79" s="18" t="s">
+      <c r="H79" s="8" t="s">
         <v>355</v>
       </c>
       <c r="I79" s="5" t="s">
@@ -7762,7 +7746,7 @@
       <c r="B80" s="16" t="n">
         <v>111</v>
       </c>
-      <c r="C80" s="27" t="s">
+      <c r="C80" s="24" t="s">
         <v>359</v>
       </c>
       <c r="D80" s="15" t="s">
@@ -7777,82 +7761,82 @@
       <c r="G80" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H80" s="28" t="s">
+      <c r="H80" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="I80" s="29" t="s">
+      <c r="I80" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="J80" s="19" t="n">
+      <c r="J80" s="18" t="n">
         <v>1.8</v>
       </c>
-      <c r="K80" s="29" t="s">
+      <c r="K80" s="26" t="s">
         <v>362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9" outlineLevel="0" r="81">
       <c r="A81" s="15"/>
       <c r="B81" s="16"/>
-      <c r="C81" s="27"/>
+      <c r="C81" s="24"/>
       <c r="D81" s="15"/>
       <c r="E81" s="17"/>
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
-      <c r="H81" s="30" t="s">
+      <c r="H81" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="I81" s="29"/>
-      <c r="J81" s="19"/>
-      <c r="K81" s="29"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="8.1" outlineLevel="0" r="82">
       <c r="A82" s="15"/>
       <c r="B82" s="16"/>
-      <c r="C82" s="27"/>
+      <c r="C82" s="24"/>
       <c r="D82" s="15"/>
       <c r="E82" s="17"/>
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
-      <c r="H82" s="30" t="s">
+      <c r="H82" s="27" t="s">
         <v>364</v>
       </c>
-      <c r="I82" s="29"/>
-      <c r="J82" s="19"/>
-      <c r="K82" s="29"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.1" outlineLevel="0" r="83">
       <c r="A83" s="15"/>
       <c r="B83" s="16"/>
-      <c r="C83" s="27"/>
+      <c r="C83" s="24"/>
       <c r="D83" s="15"/>
       <c r="E83" s="17"/>
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
-      <c r="H83" s="31" t="s">
+      <c r="H83" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="I83" s="29"/>
-      <c r="J83" s="19"/>
-      <c r="K83" s="29"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="26"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="11.1" outlineLevel="0" r="84">
       <c r="A84" s="15"/>
       <c r="B84" s="16"/>
-      <c r="C84" s="32" t="s">
+      <c r="C84" s="28" t="s">
         <v>366</v>
       </c>
       <c r="D84" s="15"/>
       <c r="E84" s="17"/>
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
-      <c r="H84" s="33" t="s">
+      <c r="H84" s="29" t="s">
         <v>367</v>
       </c>
-      <c r="I84" s="33" t="s">
+      <c r="I84" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="J84" s="19"/>
-      <c r="K84" s="33" t="s">
+      <c r="J84" s="18"/>
+      <c r="K84" s="29" t="s">
         <v>369</v>
       </c>
     </row>
@@ -7863,7 +7847,7 @@
       <c r="B85" s="16" t="n">
         <v>134</v>
       </c>
-      <c r="C85" s="23" t="s">
+      <c r="C85" s="21" t="s">
         <v>371</v>
       </c>
       <c r="D85" s="15" t="s">
@@ -7878,16 +7862,16 @@
       <c r="G85" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H85" s="24" t="s">
+      <c r="H85" s="5" t="s">
         <v>373</v>
       </c>
       <c r="I85" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="J85" s="19" t="n">
+      <c r="J85" s="18" t="n">
         <v>1.8</v>
       </c>
-      <c r="K85" s="18" t="s">
+      <c r="K85" s="8" t="s">
         <v>375</v>
       </c>
     </row>
@@ -7933,7 +7917,7 @@
       <c r="B87" s="16" t="n">
         <v>113</v>
       </c>
-      <c r="C87" s="23" t="s">
+      <c r="C87" s="21" t="s">
         <v>377</v>
       </c>
       <c r="D87" s="15" t="s">
@@ -7948,16 +7932,16 @@
       <c r="G87" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H87" s="18" t="s">
+      <c r="H87" s="8" t="s">
         <v>378</v>
       </c>
       <c r="I87" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="J87" s="19" t="n">
+      <c r="J87" s="18" t="n">
         <v>1.8</v>
       </c>
-      <c r="K87" s="18" t="s">
+      <c r="K87" s="8" t="s">
         <v>380</v>
       </c>
     </row>
@@ -7968,7 +7952,7 @@
       <c r="B88" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C88" s="23" t="s">
+      <c r="C88" s="21" t="s">
         <v>383</v>
       </c>
       <c r="D88" s="15" t="s">
@@ -7983,16 +7967,16 @@
       <c r="G88" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="H88" s="18" t="s">
+      <c r="H88" s="8" t="s">
         <v>384</v>
       </c>
       <c r="I88" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="J88" s="19" t="n">
+      <c r="J88" s="18" t="n">
         <v>1.8</v>
       </c>
-      <c r="K88" s="18" t="s">
+      <c r="K88" s="8" t="s">
         <v>386</v>
       </c>
     </row>
@@ -8003,7 +7987,7 @@
       <c r="B89" s="6" t="n">
         <v>122</v>
       </c>
-      <c r="C89" s="23" t="s">
+      <c r="C89" s="21" t="s">
         <v>388</v>
       </c>
       <c r="D89" s="5" t="s">
@@ -8018,7 +8002,7 @@
       <c r="G89" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H89" s="18" t="s">
+      <c r="H89" s="8" t="s">
         <v>389</v>
       </c>
       <c r="I89" s="5" t="s">
@@ -8074,7 +8058,7 @@
       <c r="I91" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="J91" s="34" t="n">
+      <c r="J91" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K91" s="8" t="s">
@@ -8109,7 +8093,7 @@
       <c r="I92" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="J92" s="34" t="n">
+      <c r="J92" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K92" s="8" t="s">
@@ -8144,7 +8128,7 @@
       <c r="I93" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="J93" s="34" t="n">
+      <c r="J93" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K93" s="8" t="s">
@@ -8158,7 +8142,7 @@
       <c r="B94" s="6" t="n">
         <v>98</v>
       </c>
-      <c r="C94" s="23" t="s">
+      <c r="C94" s="21" t="s">
         <v>408</v>
       </c>
       <c r="D94" s="5" t="s">
@@ -8173,13 +8157,13 @@
       <c r="G94" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="H94" s="18" t="s">
+      <c r="H94" s="8" t="s">
         <v>409</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="J94" s="35" t="n">
+      <c r="J94" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K94" s="5" t="s">
@@ -8214,7 +8198,7 @@
       <c r="I95" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="J95" s="34" t="n">
+      <c r="J95" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K95" s="8" t="s">
@@ -8225,7 +8209,7 @@
       <c r="A96" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C96" s="8" t="s">
@@ -8284,7 +8268,7 @@
       <c r="I97" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="J97" s="34" t="n">
+      <c r="J97" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K97" s="8" t="s">
@@ -8319,7 +8303,7 @@
       <c r="I98" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="J98" s="34" t="n">
+      <c r="J98" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K98" s="8" t="s">
@@ -8364,7 +8348,7 @@
       <c r="B100" s="10" t="n">
         <v>128</v>
       </c>
-      <c r="C100" s="25" t="s">
+      <c r="C100" s="22" t="s">
         <v>431</v>
       </c>
       <c r="D100" s="8" t="s">
@@ -8385,7 +8369,7 @@
       <c r="I100" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="J100" s="34" t="n">
+      <c r="J100" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K100" s="8" t="s">
@@ -8420,7 +8404,7 @@
       <c r="I101" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="J101" s="35" t="n">
+      <c r="J101" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K101" s="8" t="s">
@@ -8455,7 +8439,7 @@
       <c r="I102" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="J102" s="34" t="n">
+      <c r="J102" s="30" t="n">
         <v>1.25</v>
       </c>
       <c r="K102" s="8" t="s">
@@ -8466,7 +8450,7 @@
       <c r="A103" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C103" s="8" t="s">
@@ -8501,7 +8485,7 @@
       <c r="A104" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -8554,13 +8538,13 @@
       <c r="G105" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="H105" s="18" t="s">
+      <c r="H105" s="8" t="s">
         <v>449</v>
       </c>
       <c r="I105" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="J105" s="35" t="n">
+      <c r="J105" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K105" s="5" t="s">
@@ -8574,7 +8558,7 @@
       <c r="B106" s="6" t="n">
         <v>99</v>
       </c>
-      <c r="C106" s="23" t="s">
+      <c r="C106" s="21" t="s">
         <v>452</v>
       </c>
       <c r="D106" s="5" t="s">
@@ -8589,13 +8573,13 @@
       <c r="G106" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="H106" s="18" t="s">
+      <c r="H106" s="8" t="s">
         <v>453</v>
       </c>
       <c r="I106" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="J106" s="35" t="n">
+      <c r="J106" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K106" s="5" t="s">
@@ -8609,7 +8593,7 @@
       <c r="B107" s="16" t="n">
         <v>56</v>
       </c>
-      <c r="C107" s="23" t="s">
+      <c r="C107" s="21" t="s">
         <v>457</v>
       </c>
       <c r="D107" s="15" t="s">
@@ -8630,10 +8614,10 @@
       <c r="I107" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="J107" s="36" t="n">
+      <c r="J107" s="32" t="n">
         <v>1.25</v>
       </c>
-      <c r="K107" s="18" t="s">
+      <c r="K107" s="8" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8676,7 +8660,7 @@
       <c r="A109" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="B109" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C109" s="11" t="s">
@@ -8714,7 +8698,7 @@
       <c r="B110" s="16" t="n">
         <v>56</v>
       </c>
-      <c r="C110" s="23" t="s">
+      <c r="C110" s="21" t="s">
         <v>465</v>
       </c>
       <c r="D110" s="15" t="s">
@@ -8735,10 +8719,10 @@
       <c r="I110" s="15" t="s">
         <v>467</v>
       </c>
-      <c r="J110" s="36" t="n">
+      <c r="J110" s="32" t="n">
         <v>1.25</v>
       </c>
-      <c r="K110" s="18" t="s">
+      <c r="K110" s="8" t="s">
         <v>468</v>
       </c>
     </row>
@@ -8770,10 +8754,10 @@
       <c r="I111" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="J111" s="35" t="n">
+      <c r="J111" s="31" t="n">
         <v>1.25</v>
       </c>
-      <c r="K111" s="18" t="s">
+      <c r="K111" s="8" t="s">
         <v>475</v>
       </c>
     </row>
@@ -8890,7 +8874,7 @@
       <c r="I115" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="J115" s="34" t="n">
+      <c r="J115" s="30" t="n">
         <v>2.25</v>
       </c>
       <c r="K115" s="8" t="s">
@@ -9094,7 +9078,7 @@
       <c r="G121" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="H121" s="18" t="s">
+      <c r="H121" s="8" t="s">
         <v>519</v>
       </c>
       <c r="I121" s="5" t="s">
@@ -9114,7 +9098,7 @@
       <c r="B122" s="16" t="n">
         <v>88</v>
       </c>
-      <c r="C122" s="23" t="s">
+      <c r="C122" s="21" t="s">
         <v>523</v>
       </c>
       <c r="D122" s="15" t="s">
@@ -9129,13 +9113,13 @@
       <c r="G122" s="15" t="s">
         <v>480</v>
       </c>
-      <c r="H122" s="24" t="s">
+      <c r="H122" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="I122" s="18" t="s">
+      <c r="I122" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="J122" s="19" t="n">
+      <c r="J122" s="18" t="n">
         <v>1.5</v>
       </c>
       <c r="K122" s="8" t="s">
@@ -9319,7 +9303,7 @@
       <c r="B129" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C129" s="20" t="s">
+      <c r="C129" s="19" t="s">
         <v>478</v>
       </c>
       <c r="D129" s="5" t="s">
@@ -9874,7 +9858,7 @@
       <c r="B146" s="6" t="n">
         <v>50</v>
       </c>
-      <c r="C146" s="20" t="s">
+      <c r="C146" s="19" t="s">
         <v>478</v>
       </c>
       <c r="D146" s="5" t="s">
@@ -9892,10 +9876,10 @@
       <c r="H146" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="I146" s="18" t="s">
+      <c r="I146" s="8" t="s">
         <v>612</v>
       </c>
-      <c r="J146" s="35" t="n">
+      <c r="J146" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K146" s="8" t="s">
@@ -9924,13 +9908,13 @@
       <c r="G147" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="H147" s="18" t="s">
+      <c r="H147" s="8" t="s">
         <v>617</v>
       </c>
       <c r="I147" s="8" t="s">
         <v>618</v>
       </c>
-      <c r="J147" s="35" t="n">
+      <c r="J147" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K147" s="5" t="s">
@@ -9959,13 +9943,13 @@
       <c r="G148" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="H148" s="18" t="s">
+      <c r="H148" s="8" t="s">
         <v>622</v>
       </c>
       <c r="I148" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="J148" s="35" t="n">
+      <c r="J148" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K148" s="5" t="s">
@@ -9994,13 +9978,13 @@
       <c r="G149" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="H149" s="18" t="s">
+      <c r="H149" s="8" t="s">
         <v>628</v>
       </c>
       <c r="I149" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="J149" s="35" t="n">
+      <c r="J149" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K149" s="5" t="s">
@@ -10050,7 +10034,7 @@
       <c r="I151" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="J151" s="34" t="n">
+      <c r="J151" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K151" s="8" t="s">
@@ -10120,7 +10104,7 @@
       <c r="I153" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="J153" s="34" t="n">
+      <c r="J153" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K153" s="8" t="s">
@@ -10155,7 +10139,7 @@
       <c r="I154" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="J154" s="35" t="n">
+      <c r="J154" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K154" s="5" t="s">
@@ -10190,7 +10174,7 @@
       <c r="I155" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="J155" s="34" t="n">
+      <c r="J155" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K155" s="8" t="s">
@@ -10225,7 +10209,7 @@
       <c r="I156" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="J156" s="34" t="n">
+      <c r="J156" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K156" s="8" t="s">
@@ -10260,7 +10244,7 @@
       <c r="I157" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="J157" s="34" t="n">
+      <c r="J157" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K157" s="8" t="s">
@@ -10271,7 +10255,7 @@
       <c r="A158" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="B158" s="20" t="s">
+      <c r="B158" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C158" s="8" t="s">
@@ -10330,7 +10314,7 @@
       <c r="I159" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="J159" s="34" t="n">
+      <c r="J159" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K159" s="8" t="s">
@@ -10365,7 +10349,7 @@
       <c r="I160" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="J160" s="34" t="n">
+      <c r="J160" s="30" t="n">
         <v>0.75</v>
       </c>
       <c r="K160" s="8" t="s">
@@ -10400,7 +10384,7 @@
       <c r="I161" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="J161" s="34" t="n">
+      <c r="J161" s="30" t="n">
         <v>1.75</v>
       </c>
       <c r="K161" s="8" t="s">
@@ -10447,7 +10431,7 @@
       <c r="H163" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="I163" s="18" t="s">
+      <c r="I163" s="8" t="s">
         <v>682</v>
       </c>
       <c r="J163" s="9" t="n">
@@ -10696,19 +10680,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="172">
-      <c r="A172" s="37" t="s">
+      <c r="A172" s="33" t="s">
         <v>709</v>
       </c>
-      <c r="B172" s="37"/>
-      <c r="C172" s="37"/>
-      <c r="D172" s="37"/>
-      <c r="E172" s="37"/>
-      <c r="F172" s="37"/>
-      <c r="G172" s="37"/>
-      <c r="H172" s="37"/>
-      <c r="I172" s="37"/>
-      <c r="J172" s="37"/>
-      <c r="K172" s="37"/>
+      <c r="B172" s="33"/>
+      <c r="C172" s="33"/>
+      <c r="D172" s="33"/>
+      <c r="E172" s="33"/>
+      <c r="F172" s="33"/>
+      <c r="G172" s="33"/>
+      <c r="H172" s="33"/>
+      <c r="I172" s="33"/>
+      <c r="J172" s="33"/>
+      <c r="K172" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="173">
       <c r="A173" s="8" t="s">
@@ -10808,7 +10792,7 @@
       <c r="I175" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="J175" s="35" t="n">
+      <c r="J175" s="31" t="n">
         <v>0.75</v>
       </c>
       <c r="K175" s="5" t="s">
@@ -10843,7 +10827,7 @@
       <c r="I176" s="5" t="s">
         <v>726</v>
       </c>
-      <c r="J176" s="35" t="n">
+      <c r="J176" s="31" t="n">
         <v>1.25</v>
       </c>
       <c r="K176" s="5" t="s">
@@ -10851,19 +10835,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="177">
-      <c r="A177" s="37" t="s">
+      <c r="A177" s="33" t="s">
         <v>727</v>
       </c>
-      <c r="B177" s="37"/>
-      <c r="C177" s="37"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="37"/>
-      <c r="F177" s="37"/>
-      <c r="G177" s="37"/>
-      <c r="H177" s="37"/>
-      <c r="I177" s="37"/>
-      <c r="J177" s="37"/>
-      <c r="K177" s="37"/>
+      <c r="B177" s="33"/>
+      <c r="C177" s="33"/>
+      <c r="D177" s="33"/>
+      <c r="E177" s="33"/>
+      <c r="F177" s="33"/>
+      <c r="G177" s="33"/>
+      <c r="H177" s="33"/>
+      <c r="I177" s="33"/>
+      <c r="J177" s="33"/>
+      <c r="K177" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="178">
       <c r="A178" s="8" t="s">
@@ -10881,19 +10865,19 @@
       <c r="K178" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="179">
-      <c r="A179" s="37" t="s">
+      <c r="A179" s="33" t="s">
         <v>728</v>
       </c>
-      <c r="B179" s="37"/>
-      <c r="C179" s="37"/>
-      <c r="D179" s="37"/>
-      <c r="E179" s="37"/>
-      <c r="F179" s="37"/>
-      <c r="G179" s="37"/>
-      <c r="H179" s="37"/>
-      <c r="I179" s="37"/>
-      <c r="J179" s="37"/>
-      <c r="K179" s="37"/>
+      <c r="B179" s="33"/>
+      <c r="C179" s="33"/>
+      <c r="D179" s="33"/>
+      <c r="E179" s="33"/>
+      <c r="F179" s="33"/>
+      <c r="G179" s="33"/>
+      <c r="H179" s="33"/>
+      <c r="I179" s="33"/>
+      <c r="J179" s="33"/>
+      <c r="K179" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="180">
       <c r="A180" s="8" t="s">
@@ -11176,19 +11160,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="188">
-      <c r="A188" s="37" t="s">
+      <c r="A188" s="33" t="s">
         <v>768</v>
       </c>
-      <c r="B188" s="37"/>
-      <c r="C188" s="37"/>
-      <c r="D188" s="37"/>
-      <c r="E188" s="37"/>
-      <c r="F188" s="37"/>
-      <c r="G188" s="37"/>
-      <c r="H188" s="37"/>
-      <c r="I188" s="37"/>
-      <c r="J188" s="37"/>
-      <c r="K188" s="37"/>
+      <c r="B188" s="33"/>
+      <c r="C188" s="33"/>
+      <c r="D188" s="33"/>
+      <c r="E188" s="33"/>
+      <c r="F188" s="33"/>
+      <c r="G188" s="33"/>
+      <c r="H188" s="33"/>
+      <c r="I188" s="33"/>
+      <c r="J188" s="33"/>
+      <c r="K188" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="189">
       <c r="A189" s="8" t="s">
@@ -11366,19 +11350,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="194">
-      <c r="A194" s="37" t="s">
+      <c r="A194" s="33" t="s">
         <v>794</v>
       </c>
-      <c r="B194" s="37"/>
-      <c r="C194" s="37"/>
-      <c r="D194" s="37"/>
-      <c r="E194" s="37"/>
-      <c r="F194" s="37"/>
-      <c r="G194" s="37"/>
-      <c r="H194" s="37"/>
-      <c r="I194" s="37"/>
-      <c r="J194" s="37"/>
-      <c r="K194" s="37"/>
+      <c r="B194" s="33"/>
+      <c r="C194" s="33"/>
+      <c r="D194" s="33"/>
+      <c r="E194" s="33"/>
+      <c r="F194" s="33"/>
+      <c r="G194" s="33"/>
+      <c r="H194" s="33"/>
+      <c r="I194" s="33"/>
+      <c r="J194" s="33"/>
+      <c r="K194" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="195">
       <c r="A195" s="8" t="s">
@@ -11440,7 +11424,7 @@
       <c r="H196" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I196" s="18" t="s">
+      <c r="I196" s="8" t="s">
         <v>802</v>
       </c>
       <c r="J196" s="9" t="n">
@@ -11507,7 +11491,7 @@
       <c r="G198" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="H198" s="20" t="s">
+      <c r="H198" s="19" t="s">
         <v>17</v>
       </c>
       <c r="I198" s="5" t="s">
@@ -11551,7 +11535,7 @@
       <c r="J199" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K199" s="18" t="s">
+      <c r="K199" s="8" t="s">
         <v>813</v>
       </c>
     </row>
@@ -11577,7 +11561,7 @@
       <c r="G200" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H200" s="18" t="s">
+      <c r="H200" s="8" t="s">
         <v>817</v>
       </c>
       <c r="I200" s="5" t="s">
@@ -11621,7 +11605,7 @@
       <c r="J201" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K201" s="18" t="s">
+      <c r="K201" s="8" t="s">
         <v>824</v>
       </c>
     </row>
@@ -11702,7 +11686,7 @@
       <c r="B204" s="6" t="n">
         <v>45</v>
       </c>
-      <c r="C204" s="25" t="s">
+      <c r="C204" s="22" t="s">
         <v>834</v>
       </c>
       <c r="D204" s="5" t="s">
@@ -11737,7 +11721,7 @@
       <c r="B205" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C205" s="18" t="s">
+      <c r="C205" s="8" t="s">
         <v>839</v>
       </c>
       <c r="D205" s="5" t="s">
@@ -11766,19 +11750,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="206">
-      <c r="A206" s="37" t="s">
+      <c r="A206" s="33" t="s">
         <v>842</v>
       </c>
-      <c r="B206" s="37"/>
-      <c r="C206" s="37"/>
-      <c r="D206" s="37"/>
-      <c r="E206" s="37"/>
-      <c r="F206" s="37"/>
-      <c r="G206" s="37"/>
-      <c r="H206" s="37"/>
-      <c r="I206" s="37"/>
-      <c r="J206" s="37"/>
-      <c r="K206" s="37"/>
+      <c r="B206" s="33"/>
+      <c r="C206" s="33"/>
+      <c r="D206" s="33"/>
+      <c r="E206" s="33"/>
+      <c r="F206" s="33"/>
+      <c r="G206" s="33"/>
+      <c r="H206" s="33"/>
+      <c r="I206" s="33"/>
+      <c r="J206" s="33"/>
+      <c r="K206" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="207">
       <c r="A207" s="8" t="s">
@@ -11921,19 +11905,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="211">
-      <c r="A211" s="37" t="s">
+      <c r="A211" s="33" t="s">
         <v>864</v>
       </c>
-      <c r="B211" s="37"/>
-      <c r="C211" s="37"/>
-      <c r="D211" s="37"/>
-      <c r="E211" s="37"/>
-      <c r="F211" s="37"/>
-      <c r="G211" s="37"/>
-      <c r="H211" s="37"/>
-      <c r="I211" s="37"/>
-      <c r="J211" s="37"/>
-      <c r="K211" s="37"/>
+      <c r="B211" s="33"/>
+      <c r="C211" s="33"/>
+      <c r="D211" s="33"/>
+      <c r="E211" s="33"/>
+      <c r="F211" s="33"/>
+      <c r="G211" s="33"/>
+      <c r="H211" s="33"/>
+      <c r="I211" s="33"/>
+      <c r="J211" s="33"/>
+      <c r="K211" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="212">
       <c r="A212" s="8" t="s">
@@ -11992,7 +11976,7 @@
       <c r="G213" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="H213" s="18" t="s">
+      <c r="H213" s="8" t="s">
         <v>874</v>
       </c>
       <c r="I213" s="5" t="s">
@@ -12027,7 +12011,7 @@
       <c r="G214" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="H214" s="18" t="s">
+      <c r="H214" s="8" t="s">
         <v>874</v>
       </c>
       <c r="I214" s="5" t="s">
@@ -12041,84 +12025,84 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="215">
-      <c r="A215" s="8" t="s">
+      <c r="A215" s="34" t="s">
         <v>877</v>
       </c>
-      <c r="B215" s="10" t="n">
+      <c r="B215" s="35" t="n">
         <v>24</v>
       </c>
-      <c r="C215" s="25" t="s">
+      <c r="C215" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D215" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E215" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F215" s="34" t="s">
+        <v>845</v>
+      </c>
+      <c r="G215" s="34" t="s">
         <v>878</v>
       </c>
-      <c r="D215" s="8" t="s">
+      <c r="H215" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="I215" s="34" t="s">
+        <v>847</v>
+      </c>
+      <c r="J215" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K215" s="34" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="216">
+      <c r="A216" s="34" t="s">
+        <v>880</v>
+      </c>
+      <c r="B216" s="35" t="n">
+        <v>24</v>
+      </c>
+      <c r="C216" s="36" t="s">
+        <v>881</v>
+      </c>
+      <c r="D216" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E215" s="12" t="n">
+      <c r="E216" s="37" t="n">
         <v>6</v>
       </c>
-      <c r="F215" s="8" t="s">
+      <c r="F216" s="34" t="s">
         <v>845</v>
       </c>
-      <c r="G215" s="8" t="s">
-        <v>879</v>
-      </c>
-      <c r="H215" s="8" t="s">
+      <c r="G216" s="34" t="s">
+        <v>878</v>
+      </c>
+      <c r="H216" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="I215" s="8" t="s">
-        <v>847</v>
-      </c>
-      <c r="J215" s="14" t="n">
+      <c r="I216" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="J216" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="K215" s="8" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="216">
-      <c r="A216" s="5" t="s">
-        <v>881</v>
-      </c>
-      <c r="B216" s="5" t="s">
+      <c r="K216" s="34" t="s">
         <v>882</v>
-      </c>
-      <c r="C216" s="13" t="s">
-        <v>883</v>
-      </c>
-      <c r="D216" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E216" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F216" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="G216" s="5" t="s">
-        <v>884</v>
-      </c>
-      <c r="H216" s="5" t="s">
-        <v>885</v>
-      </c>
-      <c r="I216" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="J216" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K216" s="18" t="s">
-        <v>886</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="217">
       <c r="A217" s="5" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>882</v>
-      </c>
-      <c r="C217" s="25" t="s">
-        <v>887</v>
+        <v>884</v>
+      </c>
+      <c r="C217" s="22" t="s">
+        <v>885</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>14</v>
@@ -12130,10 +12114,10 @@
         <v>137</v>
       </c>
       <c r="G217" s="5" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="H217" s="5" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="I217" s="5" t="s">
         <v>273</v>
@@ -12141,19 +12125,19 @@
       <c r="J217" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K217" s="18" t="s">
-        <v>886</v>
+      <c r="K217" s="8" t="s">
+        <v>888</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="218">
       <c r="A218" s="8" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B218" s="12" t="n">
         <v>4</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="D218" s="8" t="s">
         <v>14</v>
@@ -12171,24 +12155,24 @@
         <v>17</v>
       </c>
       <c r="I218" s="8" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="J218" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K218" s="8" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="219">
       <c r="A219" s="8" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B219" s="8" t="s">
         <v>800</v>
       </c>
       <c r="C219" s="13" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="D219" s="8" t="s">
         <v>63</v>
@@ -12206,7 +12190,7 @@
         <v>17</v>
       </c>
       <c r="I219" s="8" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="J219" s="14" t="n">
         <v>0</v>
@@ -12217,13 +12201,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="220">
       <c r="A220" s="5" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B220" s="6" t="n">
         <v>47</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>90</v>
@@ -12235,30 +12219,30 @@
         <v>70</v>
       </c>
       <c r="G220" s="5" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="H220" s="8" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J220" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K220" s="5" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="221">
-      <c r="A221" s="18" t="s">
-        <v>901</v>
+      <c r="A221" s="8" t="s">
+        <v>902</v>
       </c>
       <c r="B221" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C221" s="20" t="s">
-        <v>902</v>
+      <c r="C221" s="19" t="s">
+        <v>903</v>
       </c>
       <c r="D221" s="5" t="s">
         <v>14</v>
@@ -12276,24 +12260,24 @@
         <v>17</v>
       </c>
       <c r="I221" s="5" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="J221" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K221" s="5" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="222">
       <c r="A222" s="5" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B222" s="6" t="n">
         <v>202</v>
       </c>
       <c r="C222" s="11" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>14</v>
@@ -12305,10 +12289,10 @@
         <v>114</v>
       </c>
       <c r="G222" s="5" t="s">
-        <v>907</v>
-      </c>
-      <c r="H222" s="18" t="s">
         <v>908</v>
+      </c>
+      <c r="H222" s="8" t="s">
+        <v>909</v>
       </c>
       <c r="I222" s="5" t="s">
         <v>273</v>
@@ -12317,7 +12301,7 @@
         <v>0</v>
       </c>
       <c r="K222" s="5" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="223">
@@ -12357,13 +12341,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="224">
       <c r="A224" s="5" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>21</v>
@@ -12377,8 +12361,8 @@
       <c r="G224" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="H224" s="18" t="s">
-        <v>913</v>
+      <c r="H224" s="8" t="s">
+        <v>914</v>
       </c>
       <c r="I224" s="5" t="s">
         <v>273</v>
@@ -12392,13 +12376,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="225">
       <c r="A225" s="5" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B225" s="6" t="n">
         <v>201</v>
       </c>
-      <c r="C225" s="25" t="s">
-        <v>915</v>
+      <c r="C225" s="22" t="s">
+        <v>916</v>
       </c>
       <c r="D225" s="5" t="s">
         <v>14</v>
@@ -12410,10 +12394,10 @@
         <v>114</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>884</v>
-      </c>
-      <c r="H225" s="18" t="s">
-        <v>916</v>
+        <v>886</v>
+      </c>
+      <c r="H225" s="8" t="s">
+        <v>917</v>
       </c>
       <c r="I225" s="5" t="s">
         <v>273</v>
@@ -12422,18 +12406,18 @@
         <v>0</v>
       </c>
       <c r="K225" s="5" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="226">
       <c r="A226" s="5" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="D226" s="5" t="s">
         <v>90</v>
@@ -12445,24 +12429,24 @@
         <v>125</v>
       </c>
       <c r="G226" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="H226" s="18" t="s">
-        <v>921</v>
+        <v>898</v>
+      </c>
+      <c r="H226" s="8" t="s">
+        <v>922</v>
       </c>
       <c r="I226" s="5" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J226" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K226" s="5" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="227">
       <c r="A227" s="8" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B227" s="11"/>
       <c r="C227" s="11"/>
@@ -12474,33 +12458,33 @@
       <c r="I227" s="11"/>
       <c r="J227" s="11"/>
       <c r="K227" s="8" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="228">
-      <c r="A228" s="37" t="s">
-        <v>925</v>
-      </c>
-      <c r="B228" s="37"/>
-      <c r="C228" s="37"/>
-      <c r="D228" s="37"/>
-      <c r="E228" s="37"/>
-      <c r="F228" s="37"/>
-      <c r="G228" s="37"/>
-      <c r="H228" s="37"/>
-      <c r="I228" s="37"/>
-      <c r="J228" s="37"/>
-      <c r="K228" s="37"/>
+      <c r="A228" s="33" t="s">
+        <v>926</v>
+      </c>
+      <c r="B228" s="33"/>
+      <c r="C228" s="33"/>
+      <c r="D228" s="33"/>
+      <c r="E228" s="33"/>
+      <c r="F228" s="33"/>
+      <c r="G228" s="33"/>
+      <c r="H228" s="33"/>
+      <c r="I228" s="33"/>
+      <c r="J228" s="33"/>
+      <c r="K228" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="229">
       <c r="A229" s="5" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B229" s="6" t="n">
         <v>14</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>14</v>
@@ -12517,25 +12501,25 @@
       <c r="H229" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I229" s="18" t="s">
-        <v>928</v>
+      <c r="I229" s="8" t="s">
+        <v>929</v>
       </c>
       <c r="J229" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K229" s="5" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="230">
       <c r="A230" s="8" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B230" s="8" t="s">
         <v>800</v>
       </c>
       <c r="C230" s="8" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="D230" s="8" t="s">
         <v>641</v>
@@ -12550,7 +12534,7 @@
         <v>273</v>
       </c>
       <c r="H230" s="8" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="I230" s="8" t="s">
         <v>273</v>
@@ -12559,12 +12543,12 @@
         <v>0</v>
       </c>
       <c r="K230" s="8" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="231">
       <c r="A231" s="8" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B231" s="8" t="s">
         <v>800</v>
@@ -12588,24 +12572,24 @@
         <v>273</v>
       </c>
       <c r="I231" s="8" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="J231" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K231" s="8" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="32.1" outlineLevel="0" r="232">
       <c r="A232" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B232" s="6" t="n">
         <v>14</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>30</v>
@@ -12620,21 +12604,21 @@
         <v>273</v>
       </c>
       <c r="H232" s="5" t="s">
-        <v>939</v>
-      </c>
-      <c r="I232" s="18" t="s">
         <v>940</v>
+      </c>
+      <c r="I232" s="8" t="s">
+        <v>941</v>
       </c>
       <c r="J232" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K232" s="5" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="233">
       <c r="A233" s="5" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>21</v>
@@ -12658,39 +12642,39 @@
         <v>273</v>
       </c>
       <c r="I233" s="5" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="J233" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K233" s="5" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="234">
-      <c r="A234" s="37" t="s">
-        <v>945</v>
-      </c>
-      <c r="B234" s="37"/>
-      <c r="C234" s="37"/>
-      <c r="D234" s="37"/>
-      <c r="E234" s="37"/>
-      <c r="F234" s="37"/>
-      <c r="G234" s="37"/>
-      <c r="H234" s="37"/>
-      <c r="I234" s="37"/>
-      <c r="J234" s="37"/>
-      <c r="K234" s="37"/>
+      <c r="A234" s="33" t="s">
+        <v>946</v>
+      </c>
+      <c r="B234" s="33"/>
+      <c r="C234" s="33"/>
+      <c r="D234" s="33"/>
+      <c r="E234" s="33"/>
+      <c r="F234" s="33"/>
+      <c r="G234" s="33"/>
+      <c r="H234" s="33"/>
+      <c r="I234" s="33"/>
+      <c r="J234" s="33"/>
+      <c r="K234" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="235">
       <c r="A235" s="5" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B235" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="C235" s="5" t="s">
         <v>947</v>
-      </c>
-      <c r="C235" s="5" t="s">
-        <v>946</v>
       </c>
       <c r="D235" s="5" t="s">
         <v>97</v>
@@ -12708,24 +12692,24 @@
         <v>273</v>
       </c>
       <c r="I235" s="5" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="J235" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K235" s="5" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="236">
       <c r="A236" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B236" s="5" t="s">
         <v>800</v>
       </c>
-      <c r="C236" s="20" t="s">
-        <v>949</v>
+      <c r="C236" s="19" t="s">
+        <v>950</v>
       </c>
       <c r="D236" s="5" t="s">
         <v>90</v>
@@ -12743,24 +12727,24 @@
         <v>800</v>
       </c>
       <c r="I236" s="8" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="J236" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K236" s="5" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="237">
       <c r="A237" s="11" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B237" s="8" t="s">
         <v>800</v>
       </c>
       <c r="C237" s="11" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="D237" s="8" t="s">
         <v>14</v>
@@ -12769,7 +12753,7 @@
         <v>1</v>
       </c>
       <c r="F237" s="8" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="G237" s="8" t="s">
         <v>273</v>
@@ -12778,24 +12762,24 @@
         <v>273</v>
       </c>
       <c r="I237" s="8" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="J237" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K237" s="8" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="238">
       <c r="A238" s="5" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B238" s="5" t="s">
         <v>800</v>
       </c>
       <c r="C238" s="13" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>641</v>
@@ -12803,8 +12787,8 @@
       <c r="E238" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="F238" s="18" t="s">
-        <v>958</v>
+      <c r="F238" s="8" t="s">
+        <v>959</v>
       </c>
       <c r="G238" s="5" t="s">
         <v>273</v>
@@ -12813,24 +12797,24 @@
         <v>273</v>
       </c>
       <c r="I238" s="5" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="J238" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K238" s="5" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="239">
       <c r="A239" s="8" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D239" s="8" t="s">
         <v>641</v>
@@ -12839,7 +12823,7 @@
         <v>0</v>
       </c>
       <c r="F239" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G239" s="8" t="s">
         <v>273</v>
@@ -12848,24 +12832,24 @@
         <v>273</v>
       </c>
       <c r="I239" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="J239" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K239" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="240">
       <c r="A240" s="8" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D240" s="8" t="s">
         <v>641</v>
@@ -12874,7 +12858,7 @@
         <v>0</v>
       </c>
       <c r="F240" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G240" s="8" t="s">
         <v>273</v>
@@ -12883,24 +12867,24 @@
         <v>273</v>
       </c>
       <c r="I240" s="8" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="J240" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K240" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="241">
       <c r="A241" s="5" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="D241" s="5" t="s">
         <v>641</v>
@@ -12909,7 +12893,7 @@
         <v>0</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G241" s="5" t="s">
         <v>273</v>
@@ -12918,24 +12902,24 @@
         <v>273</v>
       </c>
       <c r="I241" s="5" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="J241" s="9" t="n">
         <v>0</v>
       </c>
       <c r="K241" s="5" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="242">
       <c r="A242" s="8" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D242" s="8" t="s">
         <v>641</v>
@@ -12944,7 +12928,7 @@
         <v>0</v>
       </c>
       <c r="F242" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G242" s="8" t="s">
         <v>273</v>
@@ -12953,24 +12937,24 @@
         <v>273</v>
       </c>
       <c r="I242" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="J242" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K242" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="243">
       <c r="A243" s="8" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D243" s="8" t="s">
         <v>641</v>
@@ -12979,7 +12963,7 @@
         <v>0</v>
       </c>
       <c r="F243" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G243" s="8" t="s">
         <v>273</v>
@@ -12988,24 +12972,24 @@
         <v>273</v>
       </c>
       <c r="I243" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="J243" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K243" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="244">
       <c r="A244" s="8" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D244" s="8" t="s">
         <v>641</v>
@@ -13014,7 +12998,7 @@
         <v>0</v>
       </c>
       <c r="F244" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G244" s="8" t="s">
         <v>273</v>
@@ -13023,24 +13007,24 @@
         <v>273</v>
       </c>
       <c r="I244" s="8" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="J244" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K244" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="245">
       <c r="A245" s="8" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D245" s="8" t="s">
         <v>641</v>
@@ -13049,7 +13033,7 @@
         <v>0</v>
       </c>
       <c r="F245" s="8" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="G245" s="8" t="s">
         <v>273</v>
@@ -13058,29 +13042,29 @@
         <v>273</v>
       </c>
       <c r="I245" s="8" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="J245" s="14" t="n">
         <v>0</v>
       </c>
       <c r="K245" s="8" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="246">
-      <c r="A246" s="38" t="s">
-        <v>976</v>
-      </c>
-      <c r="B246" s="38"/>
-      <c r="C246" s="38"/>
-      <c r="D246" s="38"/>
-      <c r="E246" s="38"/>
-      <c r="F246" s="38"/>
-      <c r="G246" s="38"/>
-      <c r="H246" s="38"/>
-      <c r="I246" s="38"/>
-      <c r="J246" s="38"/>
-      <c r="K246" s="38"/>
+      <c r="A246" s="39" t="s">
+        <v>977</v>
+      </c>
+      <c r="B246" s="39"/>
+      <c r="C246" s="39"/>
+      <c r="D246" s="39"/>
+      <c r="E246" s="39"/>
+      <c r="F246" s="39"/>
+      <c r="G246" s="39"/>
+      <c r="H246" s="39"/>
+      <c r="I246" s="39"/>
+      <c r="J246" s="39"/>
+      <c r="K246" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>